<commit_message>
Added data, script details, and README
</commit_message>
<xml_diff>
--- a/Data/Physical_data_MS.xlsx
+++ b/Data/Physical_data_MS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Grad_school\OA_hudsonica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Grad_school\OA_hudsonica\Manuscripts\GitHub\hudsonica_transgenerational_MS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{37F9202C-DFC6-43F6-9201-2D243E5CF1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBAC81F-A65F-4C15-AD96-9050F7B3505A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{641937F3-449C-4C88-93B9-6E5A69AE1DF2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="6" xr2:uid="{641937F3-449C-4C88-93B9-6E5A69AE1DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Alkalinity_data_total_leuker200" sheetId="1" r:id="rId1"/>
@@ -507,15 +507,6 @@
     <t>AM - OWA</t>
   </si>
   <si>
-    <t>OWA_AM - OA</t>
-  </si>
-  <si>
-    <t>OWA_AM - OW</t>
-  </si>
-  <si>
-    <t>OWA_AM - OWA</t>
-  </si>
-  <si>
     <t>OA - OW</t>
   </si>
   <si>
@@ -550,6 +541,15 @@
   </si>
   <si>
     <t>OWA - AM-&gt;OWA</t>
+  </si>
+  <si>
+    <t>OWA-&gt;AM - OA</t>
+  </si>
+  <si>
+    <t>OWA-&gt;AM - OW</t>
+  </si>
+  <si>
+    <t>OWA-&gt;AM - OWA</t>
   </si>
 </sst>
 </file>
@@ -6906,7 +6906,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -8791,7 +8791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6217460-8898-41F4-A502-8A404A8875A7}">
   <dimension ref="A1:I841"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:M10"/>
     </sheetView>
   </sheetViews>
@@ -12066,7 +12066,7 @@
         <v>44000</v>
       </c>
       <c r="B194" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C194">
         <v>8.25</v>
@@ -12083,7 +12083,7 @@
         <v>44001</v>
       </c>
       <c r="B195" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C195">
         <v>8.2100000000000009</v>
@@ -12100,7 +12100,7 @@
         <v>44004</v>
       </c>
       <c r="B196" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C196">
         <v>8.23</v>
@@ -12117,7 +12117,7 @@
         <v>44006</v>
       </c>
       <c r="B197" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C197">
         <v>8.17</v>
@@ -12134,7 +12134,7 @@
         <v>44007</v>
       </c>
       <c r="B198" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C198">
         <v>8.14</v>
@@ -12151,7 +12151,7 @@
         <v>44008</v>
       </c>
       <c r="B199" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C199">
         <v>8.15</v>
@@ -12168,7 +12168,7 @@
         <v>44011</v>
       </c>
       <c r="B200" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C200">
         <v>8.1300000000000008</v>
@@ -12185,7 +12185,7 @@
         <v>44013</v>
       </c>
       <c r="B201" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C201">
         <v>8.1</v>
@@ -12202,7 +12202,7 @@
         <v>44018</v>
       </c>
       <c r="B202" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C202">
         <v>8.1300000000000008</v>
@@ -12219,7 +12219,7 @@
         <v>44020</v>
       </c>
       <c r="B203" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C203">
         <v>8.1300000000000008</v>
@@ -12236,7 +12236,7 @@
         <v>44022</v>
       </c>
       <c r="B204" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C204">
         <v>8.1300000000000008</v>
@@ -12253,7 +12253,7 @@
         <v>44025</v>
       </c>
       <c r="B205" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C205">
         <v>8.19</v>
@@ -12270,7 +12270,7 @@
         <v>44027</v>
       </c>
       <c r="B206" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C206">
         <v>8.16</v>
@@ -12287,7 +12287,7 @@
         <v>44028</v>
       </c>
       <c r="B207" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C207">
         <v>8.1300000000000008</v>
@@ -12304,7 +12304,7 @@
         <v>44032</v>
       </c>
       <c r="B208" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C208">
         <v>8.16</v>
@@ -12321,7 +12321,7 @@
         <v>44034</v>
       </c>
       <c r="B209" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C209">
         <v>8.17</v>
@@ -12338,7 +12338,7 @@
         <v>44036</v>
       </c>
       <c r="B210" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C210">
         <v>8.14</v>
@@ -12355,7 +12355,7 @@
         <v>44039</v>
       </c>
       <c r="B211" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C211">
         <v>8.16</v>
@@ -12372,7 +12372,7 @@
         <v>44041</v>
       </c>
       <c r="B212" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C212">
         <v>8.17</v>
@@ -12389,7 +12389,7 @@
         <v>44043</v>
       </c>
       <c r="B213" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C213">
         <v>8.1300000000000008</v>
@@ -12406,7 +12406,7 @@
         <v>44046</v>
       </c>
       <c r="B214" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C214">
         <v>8.17</v>
@@ -12423,7 +12423,7 @@
         <v>44048</v>
       </c>
       <c r="B215" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C215">
         <v>8.16</v>
@@ -12440,7 +12440,7 @@
         <v>44050</v>
       </c>
       <c r="B216" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C216">
         <v>8.1199999999999992</v>
@@ -12457,7 +12457,7 @@
         <v>44053</v>
       </c>
       <c r="B217" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C217">
         <v>8.15</v>
@@ -12474,7 +12474,7 @@
         <v>44055</v>
       </c>
       <c r="B218" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C218">
         <v>8.19</v>
@@ -12491,7 +12491,7 @@
         <v>44056</v>
       </c>
       <c r="B219" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C219">
         <v>8.17</v>
@@ -12508,7 +12508,7 @@
         <v>44057</v>
       </c>
       <c r="B220" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C220">
         <v>8.19</v>
@@ -12525,7 +12525,7 @@
         <v>44060</v>
       </c>
       <c r="B221" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C221">
         <v>8.2100000000000009</v>
@@ -12542,7 +12542,7 @@
         <v>44062</v>
       </c>
       <c r="B222" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C222">
         <v>8.2200000000000006</v>
@@ -12559,7 +12559,7 @@
         <v>44064</v>
       </c>
       <c r="B223" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C223">
         <v>8.23</v>
@@ -12576,7 +12576,7 @@
         <v>44067</v>
       </c>
       <c r="B224" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C224">
         <v>8.24</v>
@@ -12593,7 +12593,7 @@
         <v>44074</v>
       </c>
       <c r="B225" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C225">
         <v>8.25</v>
@@ -12610,7 +12610,7 @@
         <v>44076</v>
       </c>
       <c r="B226" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C226">
         <v>8.27</v>
@@ -12627,7 +12627,7 @@
         <v>44077</v>
       </c>
       <c r="B227" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C227">
         <v>8.25</v>
@@ -12644,7 +12644,7 @@
         <v>44083</v>
       </c>
       <c r="B228" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C228">
         <v>8.26</v>
@@ -12661,7 +12661,7 @@
         <v>44084</v>
       </c>
       <c r="B229" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C229">
         <v>8.25</v>
@@ -12678,7 +12678,7 @@
         <v>44088</v>
       </c>
       <c r="B230" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C230">
         <v>8.25</v>
@@ -12692,7 +12692,7 @@
         <v>44090</v>
       </c>
       <c r="B231" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C231">
         <v>8.26</v>
@@ -12709,7 +12709,7 @@
         <v>44091</v>
       </c>
       <c r="B232" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C232">
         <v>8.2200000000000006</v>
@@ -12726,7 +12726,7 @@
         <v>44095</v>
       </c>
       <c r="B233" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C233">
         <v>8.18</v>
@@ -12743,7 +12743,7 @@
         <v>44097</v>
       </c>
       <c r="B234" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C234">
         <v>8.2100000000000009</v>
@@ -22419,7 +22419,7 @@
         <v>44032</v>
       </c>
       <c r="B809" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C809">
         <v>7.82</v>
@@ -22436,7 +22436,7 @@
         <v>44034</v>
       </c>
       <c r="B810" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C810">
         <v>7.82</v>
@@ -22453,7 +22453,7 @@
         <v>44036</v>
       </c>
       <c r="B811" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C811">
         <v>7.83</v>
@@ -22470,7 +22470,7 @@
         <v>44039</v>
       </c>
       <c r="B812" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C812">
         <v>7.85</v>
@@ -22487,7 +22487,7 @@
         <v>44041</v>
       </c>
       <c r="B813" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C813">
         <v>7.88</v>
@@ -22504,7 +22504,7 @@
         <v>44043</v>
       </c>
       <c r="B814" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C814">
         <v>7.83</v>
@@ -22521,7 +22521,7 @@
         <v>44046</v>
       </c>
       <c r="B815" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C815">
         <v>7.85</v>
@@ -22538,7 +22538,7 @@
         <v>44048</v>
       </c>
       <c r="B816" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C816">
         <v>7.86</v>
@@ -22555,7 +22555,7 @@
         <v>44050</v>
       </c>
       <c r="B817" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C817">
         <v>7.84</v>
@@ -22572,7 +22572,7 @@
         <v>44053</v>
       </c>
       <c r="B818" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C818">
         <v>7.86</v>
@@ -22589,7 +22589,7 @@
         <v>44055</v>
       </c>
       <c r="B819" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C819">
         <v>7.85</v>
@@ -22606,7 +22606,7 @@
         <v>44056</v>
       </c>
       <c r="B820" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C820">
         <v>7.85</v>
@@ -22623,7 +22623,7 @@
         <v>44057</v>
       </c>
       <c r="B821" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C821">
         <v>7.83</v>
@@ -22640,7 +22640,7 @@
         <v>44060</v>
       </c>
       <c r="B822" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C822">
         <v>7.91</v>
@@ -22657,7 +22657,7 @@
         <v>44062</v>
       </c>
       <c r="B823" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C823">
         <v>7.78</v>
@@ -22674,7 +22674,7 @@
         <v>44064</v>
       </c>
       <c r="B824" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C824">
         <v>7.74</v>
@@ -22691,7 +22691,7 @@
         <v>44067</v>
       </c>
       <c r="B825" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C825">
         <v>7.89</v>
@@ -22708,7 +22708,7 @@
         <v>44074</v>
       </c>
       <c r="B826" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C826">
         <v>7.93</v>
@@ -22725,7 +22725,7 @@
         <v>44076</v>
       </c>
       <c r="B827" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C827">
         <v>7.83</v>
@@ -22742,7 +22742,7 @@
         <v>44077</v>
       </c>
       <c r="B828" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C828">
         <v>7.94</v>
@@ -22759,7 +22759,7 @@
         <v>44083</v>
       </c>
       <c r="B829" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C829">
         <v>7.92</v>
@@ -22776,7 +22776,7 @@
         <v>44084</v>
       </c>
       <c r="B830" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C830">
         <v>7.91</v>
@@ -22793,7 +22793,7 @@
         <v>44088</v>
       </c>
       <c r="B831" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C831">
         <v>7.91</v>
@@ -22807,7 +22807,7 @@
         <v>44090</v>
       </c>
       <c r="B832" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C832">
         <v>7.91</v>
@@ -22824,7 +22824,7 @@
         <v>44091</v>
       </c>
       <c r="B833" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C833">
         <v>7.89</v>
@@ -22841,7 +22841,7 @@
         <v>44095</v>
       </c>
       <c r="B834" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C834">
         <v>7.93</v>
@@ -22858,7 +22858,7 @@
         <v>44097</v>
       </c>
       <c r="B835" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C835">
         <v>7.87</v>
@@ -22875,7 +22875,7 @@
         <v>44098</v>
       </c>
       <c r="B836" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C836">
         <v>7.87</v>
@@ -22892,7 +22892,7 @@
         <v>44102</v>
       </c>
       <c r="B837" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C837">
         <v>7.92</v>
@@ -22909,7 +22909,7 @@
         <v>44104</v>
       </c>
       <c r="B838" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C838">
         <v>7.85</v>
@@ -22926,7 +22926,7 @@
         <v>44108</v>
       </c>
       <c r="B839" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C839">
         <v>7.92</v>
@@ -22943,7 +22943,7 @@
         <v>44112</v>
       </c>
       <c r="B840" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C840">
         <v>7.9</v>
@@ -22960,7 +22960,7 @@
         <v>44116</v>
       </c>
       <c r="B841" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C841">
         <v>7.56</v>
@@ -23040,7 +23040,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>12.451219512195101</v>
@@ -23132,7 +23132,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>15.363636363636401</v>
@@ -23796,7 +23796,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>8.1860975609756093</v>
@@ -23888,7 +23888,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>7.8590909090909102</v>
@@ -23949,7 +23949,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>0.650874728642583</v>
@@ -24029,7 +24029,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>-2.2615421227986898</v>
@@ -24049,7 +24049,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>-0.68035943517333197</v>
@@ -24069,7 +24069,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>-2.70846635167926</v>
@@ -24089,7 +24089,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>-2.8040436456996098</v>
@@ -24109,7 +24109,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>-2.9124168514412698</v>
@@ -24129,7 +24129,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>-2.02810691650593</v>
@@ -24149,7 +24149,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>-2.1236842105262799</v>
@@ -24169,7 +24169,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B13">
         <v>-2.2320574162679399</v>
@@ -24189,7 +24189,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>-9.5577294020355599E-2</v>
@@ -24209,7 +24209,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15">
         <v>-0.20395049976201399</v>
@@ -24229,7 +24229,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B16">
         <v>-0.108373205741659</v>
@@ -24256,8 +24256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6D886A-94D8-408C-AE54-1A7BA75A16A6}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24287,7 +24287,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>8.9286170348591397E-3</v>
@@ -24367,7 +24367,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>0.33593526891955999</v>
@@ -24387,7 +24387,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>0.32636071887035001</v>
@@ -24407,7 +24407,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>-7.6720725322430598E-3</v>
@@ -24427,7 +24427,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>0.33457124518613601</v>
@@ -24447,7 +24447,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>0.32700665188470102</v>
@@ -24467,7 +24467,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>-0.33403279140259301</v>
@@ -24487,7 +24487,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>8.2105263157861708E-3</v>
@@ -24507,7 +24507,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B13">
         <v>6.4593301435078598E-4</v>
@@ -24527,7 +24527,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>0.34224331771837901</v>
@@ -24547,7 +24547,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15">
         <v>0.33467872441694402</v>
@@ -24567,7 +24567,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B16">
         <v>-7.5645933014353902E-3</v>
@@ -24685,7 +24685,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B5">
         <v>662.25555555555502</v>
@@ -24705,7 +24705,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B6">
         <v>71.122222222221794</v>
@@ -24725,7 +24725,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <v>-591.13333333333298</v>

</xml_diff>